<commit_message>
Add team bid history command and enhance auction management features
</commit_message>
<xml_diff>
--- a/auction_data.xlsx
+++ b/auction_data.xlsx
@@ -9,6 +9,17 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Auction Results" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unsold Players" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CSK" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DC" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GT" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="KKR" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LSG" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MI" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PBKS" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RCB" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RR" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SRH" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,47 +468,147 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Prithvi Shaw</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>RCB</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>75L</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-11-29 13:28:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Mayank Agarawal</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>RCB</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1.1cr</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-11-29 13:32:30</t>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
         </is>
       </c>
     </row>
@@ -512,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,203 +653,255 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CSK</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>16</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>81.6cr</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>43.4cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>17</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>103.2cr</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>21.8cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>GT</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>112.1cr</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12.9cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>KKR</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>60.7cr</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>64.3cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>LSG</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>19</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>102.05cr</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>22.95cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>MI</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>20</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>122.25cr</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2.75cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PBKS</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>21</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>113.5cr</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>11.5cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>RCB</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>19</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>110.45cr</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>14.55cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>RR</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>16</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>108.95cr</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>16.05cr</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>SRH</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>15</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>99.5cr</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>25.5cr</t>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Set Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Base Price</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
         </is>
       </c>
     </row>

</xml_diff>